<commit_message>
Add  additional CSS selectors HW
</commit_message>
<xml_diff>
--- a/XPath_CSS/Xpath CSS HW.xlsx
+++ b/XPath_CSS/Xpath CSS HW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tetianavynogradska/IdeaProjects/SeleniumProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tetianavynogradska/IdeaProjects/SQL_HW/XPath_CSS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C333F7EB-D5D6-5646-9E2E-F75D59E795FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B3227B-E874-E445-AB9F-430D272CC4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{80D20B6B-926C-974E-A3A7-9C261A09135A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Element</t>
   </si>
@@ -172,16 +172,72 @@
   </si>
   <si>
     <t>Mastercard SecureCode</t>
+  </si>
+  <si>
+    <t>a[href*="+38"]</t>
+  </si>
+  <si>
+    <t>nav a[href*="contacts"]</t>
+  </si>
+  <si>
+    <t>#fat-menu</t>
+  </si>
+  <si>
+    <t>input[name = 'search']</t>
+  </si>
+  <si>
+    <t>.button.button_color_green.button_size_medium.search-form__submit.ng-star-inserted</t>
+  </si>
+  <si>
+    <t>.city-toggle__text</t>
+  </si>
+  <si>
+    <t>.top-information__inner.ng-star-inserted</t>
+  </si>
+  <si>
+    <t>rz-user&gt;.header__button.ng-star-inserted</t>
+  </si>
+  <si>
+    <t>rz-cart&gt;.header__button.ng-star-inserted</t>
+  </si>
+  <si>
+    <t>.premium-wrapper.ng-star-inserted</t>
+  </si>
+  <si>
+    <t>.main-slider__pagination-link</t>
+  </si>
+  <si>
+    <t>.button.button--navy</t>
+  </si>
+  <si>
+    <t>button[title = 'MasterCard Secure']</t>
+  </si>
+  <si>
+    <t>a[title = "Приложение для Андроида"]</t>
+  </si>
+  <si>
+    <t>a[title = "Приложение для Айфона"]</t>
+  </si>
+  <si>
+    <t>a[href="https://rozetka.com.ua/cabinet/orders/"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -231,10 +287,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -249,8 +306,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -278,8 +337,8 @@
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>186722</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>349380</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -632,7 +691,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,7 +735,9 @@
       <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -692,7 +753,9 @@
       <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -706,7 +769,9 @@
       <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -720,7 +785,9 @@
       <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -734,9 +801,11 @@
       <c r="E6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="F6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -748,7 +817,9 @@
       <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -758,11 +829,15 @@
         <v>9</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -778,7 +853,9 @@
       <c r="E9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -792,7 +869,9 @@
       <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -806,7 +885,9 @@
       <c r="E11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -822,7 +903,9 @@
       <c r="E12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -838,7 +921,9 @@
       <c r="E13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -852,7 +937,9 @@
       <c r="E14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -868,7 +955,9 @@
       <c r="E15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -882,7 +971,9 @@
       <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -896,10 +987,12 @@
       <c r="E17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -916,7 +1009,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{9511B403-E5DC-1543-B707-764E1FA89FEB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>